<commit_message>
new names in comparison to yesterday
</commit_message>
<xml_diff>
--- a/output/agencycount_compare.xlsx
+++ b/output/agencycount_compare.xlsx
@@ -405,10 +405,10 @@
         <v>9</v>
       </c>
       <c r="C3">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4">
@@ -469,10 +469,10 @@
         <v>27</v>
       </c>
       <c r="C7">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D7">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8">
@@ -485,10 +485,10 @@
         <v>23</v>
       </c>
       <c r="C8">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D8">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9">
@@ -517,10 +517,10 @@
         <v>35</v>
       </c>
       <c r="C10">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D10">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11">
@@ -581,10 +581,10 @@
         <v>26</v>
       </c>
       <c r="C14">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15">
@@ -613,10 +613,10 @@
         <v>13</v>
       </c>
       <c r="C16">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D16">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17">
@@ -629,10 +629,10 @@
         <v>29</v>
       </c>
       <c r="C17">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D17">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18">
@@ -645,10 +645,10 @@
         <v>20</v>
       </c>
       <c r="C18">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D18">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19">
@@ -821,10 +821,10 @@
         <v>18</v>
       </c>
       <c r="C29">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D29">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="30">
@@ -837,10 +837,10 @@
         <v>10</v>
       </c>
       <c r="C30">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D30">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31">
@@ -917,10 +917,10 @@
         <v>17</v>
       </c>
       <c r="C35">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D35">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36">
@@ -965,10 +965,10 @@
         <v>20</v>
       </c>
       <c r="C38">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D38">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39">

</xml_diff>

<commit_message>
updated data, includes new on_multiple_teams field
</commit_message>
<xml_diff>
--- a/output/agencycount_compare.xlsx
+++ b/output/agencycount_compare.xlsx
@@ -386,13 +386,13 @@
         </is>
       </c>
       <c r="B2">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C2">
         <v>7</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3">
@@ -402,13 +402,13 @@
         </is>
       </c>
       <c r="B3">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C3">
         <v>9</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4">
@@ -498,13 +498,13 @@
         </is>
       </c>
       <c r="B9">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C9">
         <v>20</v>
       </c>
       <c r="D9">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10">
@@ -514,13 +514,13 @@
         </is>
       </c>
       <c r="B10">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C10">
         <v>40</v>
       </c>
       <c r="D10">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11">
@@ -530,13 +530,13 @@
         </is>
       </c>
       <c r="B11">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C11">
         <v>31</v>
       </c>
       <c r="D11">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12">
@@ -546,13 +546,13 @@
         </is>
       </c>
       <c r="B12">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C12">
         <v>20</v>
       </c>
       <c r="D12">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13">
@@ -578,13 +578,13 @@
         </is>
       </c>
       <c r="B14">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C14">
         <v>26</v>
       </c>
       <c r="D14">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15">
@@ -594,13 +594,13 @@
         </is>
       </c>
       <c r="B15">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C15">
         <v>30</v>
       </c>
       <c r="D15">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16">
@@ -658,13 +658,13 @@
         </is>
       </c>
       <c r="B19">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C19">
         <v>14</v>
       </c>
       <c r="D19">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20">
@@ -674,13 +674,13 @@
         </is>
       </c>
       <c r="B20">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C20">
         <v>12</v>
       </c>
       <c r="D20">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21">
@@ -770,13 +770,13 @@
         </is>
       </c>
       <c r="B26">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C26">
         <v>24</v>
       </c>
       <c r="D26">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27">
@@ -786,13 +786,13 @@
         </is>
       </c>
       <c r="B27">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C27">
         <v>16</v>
       </c>
       <c r="D27">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="28">
@@ -914,13 +914,13 @@
         </is>
       </c>
       <c r="B35">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C35">
         <v>17</v>
       </c>
       <c r="D35">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36">

</xml_diff>

<commit_message>
updated with new data from Nov 30
</commit_message>
<xml_diff>
--- a/output/agencycount_compare.xlsx
+++ b/output/agencycount_compare.xlsx
@@ -514,13 +514,13 @@
         </is>
       </c>
       <c r="B10">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C10">
         <v>43</v>
       </c>
       <c r="D10">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11">
@@ -770,13 +770,13 @@
         </is>
       </c>
       <c r="B26">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C26">
         <v>25</v>
       </c>
       <c r="D26">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27">

</xml_diff>

<commit_message>
changed reference file for archive to reflect changes since early am Dec 1
</commit_message>
<xml_diff>
--- a/output/agencycount_compare.xlsx
+++ b/output/agencycount_compare.xlsx
@@ -517,10 +517,10 @@
         <v>44</v>
       </c>
       <c r="C10">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D10">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
@@ -773,10 +773,10 @@
         <v>26</v>
       </c>
       <c r="C26">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D26">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27">

</xml_diff>

<commit_message>
updated data pointing to new archived reference file
</commit_message>
<xml_diff>
--- a/output/agencycount_compare.xlsx
+++ b/output/agencycount_compare.xlsx
@@ -453,10 +453,10 @@
         <v>27</v>
       </c>
       <c r="C6">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D6">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
@@ -517,10 +517,10 @@
         <v>45</v>
       </c>
       <c r="C10">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D10">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
@@ -533,10 +533,10 @@
         <v>38</v>
       </c>
       <c r="C11">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D11">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12">
@@ -565,10 +565,10 @@
         <v>32</v>
       </c>
       <c r="C13">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="D13">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14">
@@ -693,10 +693,10 @@
         <v>6</v>
       </c>
       <c r="C21">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D21">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22">
@@ -821,10 +821,10 @@
         <v>19</v>
       </c>
       <c r="C29">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D29">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30">
@@ -869,10 +869,10 @@
         <v>11</v>
       </c>
       <c r="C32">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D32">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33">
@@ -917,10 +917,10 @@
         <v>19</v>
       </c>
       <c r="C35">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D35">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36">
@@ -997,10 +997,10 @@
         <v>10</v>
       </c>
       <c r="C40">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D40">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41">
@@ -1013,10 +1013,10 @@
         <v>5</v>
       </c>
       <c r="C41">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D41">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated data for Dec 8
</commit_message>
<xml_diff>
--- a/output/agencycount_compare.xlsx
+++ b/output/agencycount_compare.xlsx
@@ -594,13 +594,13 @@
         </is>
       </c>
       <c r="B15">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C15">
         <v>31</v>
       </c>
       <c r="D15">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16">
@@ -690,13 +690,13 @@
         </is>
       </c>
       <c r="B21">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C21">
         <v>6</v>
       </c>
       <c r="D21">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22">
@@ -786,13 +786,13 @@
         </is>
       </c>
       <c r="B27">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C27">
         <v>19</v>
       </c>
       <c r="D27">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28">
@@ -818,13 +818,13 @@
         </is>
       </c>
       <c r="B29">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C29">
         <v>19</v>
       </c>
       <c r="D29">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30">

</xml_diff>

<commit_message>
reset with new archived snapshot file
</commit_message>
<xml_diff>
--- a/output/agencycount_compare.xlsx
+++ b/output/agencycount_compare.xlsx
@@ -597,10 +597,10 @@
         <v>32</v>
       </c>
       <c r="C15">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D15">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16">
@@ -693,10 +693,10 @@
         <v>7</v>
       </c>
       <c r="C21">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D21">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22">
@@ -789,10 +789,10 @@
         <v>20</v>
       </c>
       <c r="C27">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D27">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28">
@@ -821,10 +821,10 @@
         <v>20</v>
       </c>
       <c r="C29">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D29">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30">

</xml_diff>

<commit_message>
updated with new names as of Dec 16
</commit_message>
<xml_diff>
--- a/output/agencycount_compare.xlsx
+++ b/output/agencycount_compare.xlsx
@@ -389,10 +389,10 @@
         <v>9</v>
       </c>
       <c r="C2">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -437,10 +437,10 @@
         <v>5</v>
       </c>
       <c r="C5">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -453,10 +453,10 @@
         <v>28</v>
       </c>
       <c r="C6">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D6">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
@@ -485,10 +485,10 @@
         <v>25</v>
       </c>
       <c r="C8">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D8">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
@@ -498,13 +498,13 @@
         </is>
       </c>
       <c r="B9">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C9">
         <v>21</v>
       </c>
       <c r="D9">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10">
@@ -517,10 +517,10 @@
         <v>48</v>
       </c>
       <c r="C10">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="D10">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
@@ -546,13 +546,13 @@
         </is>
       </c>
       <c r="B12">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C12">
         <v>21</v>
       </c>
       <c r="D12">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13">
@@ -562,13 +562,13 @@
         </is>
       </c>
       <c r="B13">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C13">
         <v>32</v>
       </c>
       <c r="D13">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14">
@@ -610,13 +610,13 @@
         </is>
       </c>
       <c r="B16">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C16">
         <v>13</v>
       </c>
       <c r="D16">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17">
@@ -626,13 +626,13 @@
         </is>
       </c>
       <c r="B17">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C17">
         <v>29</v>
       </c>
       <c r="D17">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18">
@@ -642,13 +642,13 @@
         </is>
       </c>
       <c r="B18">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C18">
         <v>21</v>
       </c>
       <c r="D18">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19">
@@ -661,10 +661,10 @@
         <v>16</v>
       </c>
       <c r="C19">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D19">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20">
@@ -674,13 +674,13 @@
         </is>
       </c>
       <c r="B20">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C20">
         <v>13</v>
       </c>
       <c r="D20">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21">
@@ -709,10 +709,10 @@
         <v>5</v>
       </c>
       <c r="C22">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D22">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23">
@@ -866,13 +866,13 @@
         </is>
       </c>
       <c r="B32">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C32">
         <v>11</v>
       </c>
       <c r="D32">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33">
@@ -962,10 +962,10 @@
         </is>
       </c>
       <c r="B38">
+        <v>22</v>
+      </c>
+      <c r="C38">
         <v>21</v>
-      </c>
-      <c r="C38">
-        <v>20</v>
       </c>
       <c r="D38">
         <v>1</v>

</xml_diff>

<commit_message>
updated with new names as of Dec 21 am
</commit_message>
<xml_diff>
--- a/output/agencycount_compare.xlsx
+++ b/output/agencycount_compare.xlsx
@@ -482,13 +482,13 @@
         </is>
       </c>
       <c r="B8">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C8">
         <v>25</v>
       </c>
       <c r="D8">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9">
@@ -514,13 +514,13 @@
         </is>
       </c>
       <c r="B10">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C10">
         <v>48</v>
       </c>
       <c r="D10">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11">
@@ -530,13 +530,13 @@
         </is>
       </c>
       <c r="B11">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C11">
         <v>38</v>
       </c>
       <c r="D11">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12">
@@ -690,13 +690,13 @@
         </is>
       </c>
       <c r="B21">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C21">
         <v>7</v>
       </c>
       <c r="D21">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="22">
@@ -770,13 +770,13 @@
         </is>
       </c>
       <c r="B26">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C26">
         <v>26</v>
       </c>
       <c r="D26">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27">
@@ -786,13 +786,13 @@
         </is>
       </c>
       <c r="B27">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C27">
         <v>20</v>
       </c>
       <c r="D27">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28">

</xml_diff>

<commit_message>
updated data and reset archive
</commit_message>
<xml_diff>
--- a/output/agencycount_compare.xlsx
+++ b/output/agencycount_compare.xlsx
@@ -450,13 +450,13 @@
         </is>
       </c>
       <c r="B6">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C6">
         <v>28</v>
       </c>
       <c r="D6">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7">
@@ -466,13 +466,13 @@
         </is>
       </c>
       <c r="B7">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C7">
         <v>38</v>
       </c>
       <c r="D7">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8">
@@ -482,13 +482,13 @@
         </is>
       </c>
       <c r="B8">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C8">
         <v>26</v>
       </c>
       <c r="D8">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9">
@@ -514,13 +514,13 @@
         </is>
       </c>
       <c r="B10">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C10">
         <v>50</v>
       </c>
       <c r="D10">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11">
@@ -578,13 +578,13 @@
         </is>
       </c>
       <c r="B14">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C14">
         <v>29</v>
       </c>
       <c r="D14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15">
@@ -594,13 +594,13 @@
         </is>
       </c>
       <c r="B15">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C15">
         <v>32</v>
       </c>
       <c r="D15">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16">
@@ -690,13 +690,13 @@
         </is>
       </c>
       <c r="B21">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C21">
         <v>10</v>
       </c>
       <c r="D21">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22">
@@ -770,13 +770,13 @@
         </is>
       </c>
       <c r="B26">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C26">
         <v>27</v>
       </c>
       <c r="D26">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27">
@@ -914,13 +914,13 @@
         </is>
       </c>
       <c r="B35">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C35">
         <v>19</v>
       </c>
       <c r="D35">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36">
@@ -962,13 +962,13 @@
         </is>
       </c>
       <c r="B38">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C38">
         <v>22</v>
       </c>
       <c r="D38">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39">
@@ -978,13 +978,13 @@
         </is>
       </c>
       <c r="B39">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C39">
         <v>2</v>
       </c>
       <c r="D39">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="40">

</xml_diff>